<commit_message>
Applied Dorongon's IMprovements (tysm sa pag clean ng code ko)
</commit_message>
<xml_diff>
--- a/sale.xlsx
+++ b/sale.xlsx
@@ -270,7 +270,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
@@ -688,27 +688,51 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="n">
+      <c r="A22" s="2" t="n">
         <v>2715</v>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B22" s="2" t="inlineStr">
         <is>
           <t>2026-01-20 17:04:51</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>A001</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
+      <c r="C22" s="2" t="inlineStr">
+        <is>
+          <t>A001</t>
+        </is>
+      </c>
+      <c r="D22" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E22" t="n">
-        <v>154.25</v>
-      </c>
-      <c r="F22" t="n">
-        <v>154.25</v>
+      <c r="E22" s="2" t="n">
+        <v>154.25</v>
+      </c>
+      <c r="F22" s="2" t="n">
+        <v>154.25</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2026-01-21 13:31:40</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>A001</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>2</v>
+      </c>
+      <c r="E23" t="n">
+        <v>154.25</v>
+      </c>
+      <c r="F23" t="n">
+        <v>308.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>